<commit_message>
Published state of ETDataset on 29 October 2015
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/transport/transport_truck_using_diesel_mix.converter.xlsx
+++ b/nodes_source_analyses/transport/transport_truck_using_diesel_mix.converter.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robterwel/Projects/etdataset/nodes_source_analyses/transport/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23460" tabRatio="762" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -31,7 +36,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>Source</t>
   </si>
@@ -297,6 +302,21 @@
       </rPr>
       <t>.truck_kms</t>
     </r>
+  </si>
+  <si>
+    <t>MJ/km</t>
+  </si>
+  <si>
+    <t>km/MJ</t>
+  </si>
+  <si>
+    <t>p.66</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>efficiency</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1069,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1080,7 +1100,6 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1239,6 +1258,19 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="245">
@@ -1490,6 +1522,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1525,7 +1562,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1533,6 +1570,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -1677,11 +1720,49 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4165600" y="12534900"/>
+          <a:ext cx="7302500" cy="3403600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -2122,32 +2203,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="17" customWidth="1"/>
-    <col min="4" max="16384" width="10.625" style="17"/>
+    <col min="1" max="1" width="3.1640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="23" customFormat="1">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:3" ht="20">
+    <row r="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -2156,7 +2237,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -2165,7 +2246,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -2174,128 +2255,123 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="62"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="61"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="64" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1">
+    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="66" t="s">
+      <c r="B13" s="62"/>
+      <c r="C13" s="65" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="63" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="68" t="s">
+      <c r="B17" s="62"/>
+      <c r="C17" s="67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="69" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="68" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="62"/>
+      <c r="C19" s="69" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="72" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="71" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="73" t="s">
+      <c r="B21" s="70"/>
+      <c r="C21" s="72" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="74" t="s">
+      <c r="B22" s="70"/>
+      <c r="C22" s="73" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="71"/>
-      <c r="C23" s="75" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="70"/>
+      <c r="C23" s="74" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2306,70 +2382,70 @@
   </sheetPr>
   <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="30" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="30" customWidth="1"/>
-    <col min="3" max="3" width="33.875" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="30" customWidth="1"/>
-    <col min="5" max="5" width="17.375" style="30" customWidth="1"/>
-    <col min="6" max="6" width="4.625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="44.25" style="30" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="30" customWidth="1"/>
-    <col min="9" max="9" width="42.5" style="30" customWidth="1"/>
-    <col min="10" max="10" width="3.75" style="30" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="30"/>
+    <col min="1" max="1" width="3.1640625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="44.1640625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="29" customWidth="1"/>
+    <col min="9" max="9" width="42.5" style="29" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="2:11">
-      <c r="B2" s="115" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="118"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="118"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row r="6" spans="2:11" ht="16" thickBot="1">
-      <c r="D6" s="31"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="32"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="117"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="117"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="120"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="30"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="31"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2377,33 +2453,33 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="2:11" s="20" customFormat="1">
-      <c r="B8" s="76"/>
-      <c r="C8" s="77" t="s">
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="2:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="75"/>
+      <c r="C8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77" t="s">
+      <c r="F8" s="76"/>
+      <c r="G8" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77" t="s">
+      <c r="H8" s="76"/>
+      <c r="I8" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="79"/>
-    </row>
-    <row r="9" spans="2:11" s="20" customFormat="1">
-      <c r="B9" s="19"/>
+      <c r="J8" s="78"/>
+    </row>
+    <row r="9" spans="2:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="27"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2411,12 +2487,12 @@
       <c r="I9" s="13"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="2:11" s="20" customFormat="1" ht="16" thickBot="1">
-      <c r="B10" s="19"/>
+    <row r="10" spans="2:11" s="19" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
       <c r="C10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -2424,170 +2500,173 @@
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="2:11" s="20" customFormat="1" ht="16" thickBot="1">
-      <c r="B11" s="19"/>
-      <c r="C11" s="114" t="s">
+    <row r="11" spans="2:11" s="19" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="29">
-        <v>0.409500409500409</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="29" t="s">
-        <v>27</v>
+      <c r="D11" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="28">
+        <f>'Research data'!G7</f>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="127" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="128" t="s">
+        <v>57</v>
       </c>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="35"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="2:11" ht="16" thickBot="1">
-      <c r="B13" s="35"/>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="34"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34"/>
       <c r="C13" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="2:11" ht="16" thickBot="1">
-      <c r="B14" s="35"/>
-      <c r="C14" s="34" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34"/>
+      <c r="C14" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="36">
-        <f>'Research data'!G10</f>
+      <c r="E14" s="35">
+        <f>'Research data'!G13</f>
         <v>86176</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34" t="s">
+      <c r="F14" s="33"/>
+      <c r="G14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="104" t="s">
+      <c r="H14" s="33"/>
+      <c r="I14" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="83"/>
-    </row>
-    <row r="15" spans="2:11" ht="16" thickBot="1">
-      <c r="B15" s="35"/>
-      <c r="C15" s="34" t="s">
+      <c r="J14" s="82"/>
+    </row>
+    <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34"/>
+      <c r="C15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="84">
-        <f>'Research data'!G11</f>
+      <c r="E15" s="83">
+        <f>'Research data'!G14</f>
         <v>3640</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34" t="s">
+      <c r="F15" s="33"/>
+      <c r="G15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="66" t="s">
+      <c r="H15" s="33"/>
+      <c r="I15" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="83"/>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="B16" s="35"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="83"/>
-    </row>
-    <row r="17" spans="2:10" ht="16" thickBot="1">
-      <c r="B17" s="35"/>
+      <c r="J15" s="82"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="34"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="82"/>
+    </row>
+    <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
       <c r="C17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="83"/>
-    </row>
-    <row r="18" spans="2:10" ht="16" thickBot="1">
-      <c r="B18" s="35"/>
-      <c r="C18" s="34" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="82"/>
+    </row>
+    <row r="18" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34"/>
+      <c r="C18" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="36">
-        <f>'Research data'!G7</f>
+      <c r="E18" s="35">
+        <f>'Research data'!G10</f>
         <v>12</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="59" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="106" t="s">
+      <c r="H18" s="33"/>
+      <c r="I18" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="83"/>
-    </row>
-    <row r="19" spans="2:10" ht="16" thickBot="1">
-      <c r="B19" s="35"/>
-      <c r="C19" s="34" t="s">
+      <c r="J18" s="82"/>
+    </row>
+    <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="35">
         <v>0</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="29" t="s">
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="83"/>
-    </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
+      <c r="J19" s="82"/>
+    </row>
+    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2627,11 +2706,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2640,86 +2714,86 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:M11"/>
+  <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="40" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="40" customWidth="1"/>
-    <col min="3" max="3" width="33.125" style="40" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="40" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="40" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="40" customWidth="1"/>
-    <col min="7" max="7" width="9.625" style="40" customWidth="1"/>
-    <col min="8" max="8" width="2.625" style="40" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="40" customWidth="1"/>
-    <col min="10" max="10" width="2.125" style="40" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="40" customWidth="1"/>
-    <col min="12" max="12" width="2.875" style="40" customWidth="1"/>
-    <col min="13" max="13" width="59.125" style="40" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="40"/>
+    <col min="1" max="1" width="4.33203125" style="39" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="39" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="39" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="39" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="39" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="39" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="39" customWidth="1"/>
+    <col min="10" max="10" width="2.1640625" style="39" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="39" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="39" customWidth="1"/>
+    <col min="13" max="13" width="59.1640625" style="39" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="39"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="16" thickBot="1"/>
-    <row r="3" spans="2:13">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-    </row>
-    <row r="4" spans="2:13" s="20" customFormat="1">
-      <c r="B4" s="19"/>
-      <c r="C4" s="88" t="s">
+    <row r="2" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="18"/>
+      <c r="C4" s="87" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88" t="s">
+      <c r="H4" s="87"/>
+      <c r="I4" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88" t="s">
+      <c r="J4" s="87"/>
+      <c r="K4" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="87"/>
+      <c r="M4" s="87" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="18" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="M5" s="56"/>
-    </row>
-    <row r="6" spans="2:13" ht="18" customHeight="1" thickBot="1">
-      <c r="B6" s="43"/>
+    <row r="5" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="42"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
       <c r="C6" s="12" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -2727,126 +2801,168 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="55"/>
-    </row>
-    <row r="7" spans="2:13" ht="16" thickBot="1">
-      <c r="B7" s="43"/>
-      <c r="C7" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="51">
-        <f>ROUND(12,0)</f>
-        <v>12</v>
-      </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="51">
-        <f>Notes!C12</f>
-        <v>12</v>
-      </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="58"/>
-    </row>
-    <row r="8" spans="2:13">
-      <c r="B8" s="43"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="46"/>
-    </row>
-    <row r="9" spans="2:13" ht="16" thickBot="1">
-      <c r="B9" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="54"/>
+    </row>
+    <row r="7" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
+      <c r="C7" s="124" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="125" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="126">
+        <f>K7</f>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="126">
+        <f>Notes!E70</f>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="L7" s="43"/>
+      <c r="M7" s="57"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="42"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="M8" s="55"/>
+    </row>
+    <row r="9" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="42"/>
       <c r="C9" s="12" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="60"/>
-    </row>
-    <row r="10" spans="2:13" ht="16" thickBot="1">
-      <c r="B10" s="43"/>
-      <c r="C10" s="87" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="54"/>
+    </row>
+    <row r="10" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
+      <c r="C10" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="50">
+        <f>ROUND(12,0)</f>
+        <v>12</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="50">
+        <f>Notes!C12</f>
+        <v>12</v>
+      </c>
+      <c r="L10" s="43"/>
+      <c r="M10" s="57"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="42"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="45"/>
+    </row>
+    <row r="12" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="59"/>
+    </row>
+    <row r="13" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="57" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="48">
-        <f>ROUND(AVERAGE(I10,K10),2)</f>
+      <c r="G13" s="47">
+        <f>ROUND(AVERAGE(I13,K13),2)</f>
         <v>86176</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="86">
+      <c r="H13" s="11"/>
+      <c r="I13" s="85">
         <f>Notes!C47</f>
         <v>74052</v>
       </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="48">
+      <c r="J13" s="43"/>
+      <c r="K13" s="47">
         <f>Notes!C29</f>
         <v>98300</v>
       </c>
-      <c r="L10" s="44"/>
-      <c r="M10" s="89"/>
-    </row>
-    <row r="11" spans="2:13" ht="16" thickBot="1">
-      <c r="B11" s="43"/>
-      <c r="C11" s="87" t="s">
+      <c r="L13" s="43"/>
+      <c r="M13" s="88"/>
+    </row>
+    <row r="14" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="85" t="s">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G14" s="52">
         <f>ROUND(3640,2)</f>
         <v>3640</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="53">
+      <c r="H14" s="53"/>
+      <c r="I14" s="52">
         <f>Notes!C54+Notes!C55</f>
         <v>3640</v>
       </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="89" t="s">
+      <c r="J14" s="43"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="88" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2857,38 +2973,38 @@
   </sheetPr>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="90" customWidth="1"/>
-    <col min="2" max="2" width="4" style="90" customWidth="1"/>
-    <col min="3" max="3" width="27.875" style="90" customWidth="1"/>
-    <col min="4" max="4" width="16.125" style="90" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="90" customWidth="1"/>
-    <col min="6" max="7" width="13.25" style="90" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="91" customWidth="1"/>
-    <col min="9" max="9" width="32.75" style="91" customWidth="1"/>
-    <col min="10" max="10" width="98.375" style="90" customWidth="1"/>
-    <col min="11" max="16384" width="33.125" style="90"/>
+    <col min="1" max="1" width="3.1640625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="4" style="89" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="89" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="89" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="89" customWidth="1"/>
+    <col min="6" max="7" width="13.1640625" style="89" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="90" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" style="90" customWidth="1"/>
+    <col min="10" max="10" width="98.33203125" style="89" customWidth="1"/>
+    <col min="11" max="16384" width="33.1640625" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="16" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="B2" s="92"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="93"/>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="95"/>
+    <row r="1" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="92"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="94"/>
       <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
@@ -2896,972 +3012,1088 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="97"/>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="95"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="97"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="99"/>
-      <c r="C5" s="77" t="s">
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="96"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="94"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="96"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="98"/>
+      <c r="C5" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="100" t="s">
+      <c r="I5" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="77" t="s">
+      <c r="J5" s="76" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="95"/>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="94"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="95"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="97" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="94"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="97">
+      <c r="F7" s="96">
         <v>2013</v>
       </c>
-      <c r="G7" s="97">
+      <c r="G7" s="96">
         <v>2012</v>
       </c>
-      <c r="H7" s="102"/>
-      <c r="I7" s="113" t="s">
+      <c r="H7" s="101"/>
+      <c r="I7" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="112" t="s">
+      <c r="J7" s="111" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="95"/>
-      <c r="C8" s="103" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="94"/>
+      <c r="C8" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="97"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="97"/>
-      <c r="J8" s="97"/>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="95"/>
-      <c r="C9" s="101" t="s">
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="94"/>
+      <c r="C9" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="97"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="97"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="95"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="95"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="97" t="s">
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="94"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="94"/>
+      <c r="C11" s="129" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="96">
         <v>2013</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="96">
         <v>2012</v>
       </c>
-      <c r="H11" s="97"/>
-      <c r="I11" s="113" t="s">
+      <c r="H11" s="96"/>
+      <c r="I11" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="96" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="95"/>
-      <c r="C12" s="101" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="94"/>
+      <c r="C12" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="95"/>
-      <c r="C13" s="101" t="s">
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="94"/>
+      <c r="C13" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K62"/>
+  <dimension ref="B1:K97"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69:C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.625" style="107" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="107" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="107" customWidth="1"/>
-    <col min="4" max="10" width="10.625" style="107"/>
-    <col min="11" max="11" width="10" style="107" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="107"/>
+    <col min="1" max="1" width="5.6640625" style="106" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="106" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="106" customWidth="1"/>
+    <col min="4" max="10" width="10.83203125" style="106"/>
+    <col min="11" max="11" width="10" style="106" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1"/>
-    <row r="2" spans="2:11">
-      <c r="B2" s="108"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-    </row>
-    <row r="3" spans="2:11" s="20" customFormat="1">
-      <c r="B3" s="76"/>
-      <c r="C3" s="77" t="s">
+    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="107"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+    </row>
+    <row r="3" spans="2:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="75"/>
+      <c r="C3" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="110"/>
-      <c r="C6" s="111" t="s">
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="109"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="109"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="109"/>
+      <c r="C6" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="110"/>
-      <c r="C7" s="111" t="s">
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="109"/>
+      <c r="C7" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="110"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="110"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="110"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="111"/>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="110"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="110"/>
-      <c r="C12" s="111">
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="109"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="109"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="109"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
+      <c r="K10" s="110"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="110"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="109"/>
+      <c r="C12" s="110">
         <v>12</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="110"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="110"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="111"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="111"/>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="110"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="111"/>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="B16" s="110"/>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="B17" s="110"/>
-      <c r="C17" s="111"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="111"/>
-    </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="110"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-    </row>
-    <row r="19" spans="2:11">
-      <c r="B19" s="110"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="111"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="110"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
-      <c r="K20" s="111"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="110"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="110"/>
-      <c r="C22" s="111" t="s">
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="110"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="110"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="110"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="110"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="109"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="110"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="109"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="109"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
+      <c r="G21" s="110"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="110"/>
+      <c r="K21" s="110"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="109"/>
+      <c r="C22" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="111"/>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111"/>
-      <c r="J22" s="111"/>
-      <c r="K22" s="111"/>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="110"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="110"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-    </row>
-    <row r="25" spans="2:11">
-      <c r="B25" s="110"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="111"/>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="110"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="111"/>
-    </row>
-    <row r="27" spans="2:11">
-      <c r="B27" s="110"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-    </row>
-    <row r="28" spans="2:11">
-      <c r="B28" s="110"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="111"/>
-    </row>
-    <row r="29" spans="2:11">
-      <c r="B29" s="110"/>
-      <c r="C29" s="111">
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="110"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="110"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="109"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="110"/>
+      <c r="J24" s="110"/>
+      <c r="K24" s="110"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="109"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
+      <c r="J25" s="110"/>
+      <c r="K25" s="110"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="109"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="110"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="109"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="109"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="110"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="109"/>
+      <c r="C29" s="110">
         <v>98300</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="111"/>
-      <c r="I29" s="111"/>
-      <c r="J29" s="111"/>
-      <c r="K29" s="111"/>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="110"/>
-      <c r="C30" s="111"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
-      <c r="I30" s="111"/>
-      <c r="J30" s="111"/>
-      <c r="K30" s="111"/>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="B31" s="110"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="111"/>
-      <c r="H31" s="111"/>
-      <c r="I31" s="111"/>
-      <c r="J31" s="111"/>
-      <c r="K31" s="111"/>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="110"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="111"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="111"/>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="111"/>
-    </row>
-    <row r="33" spans="2:11">
-      <c r="B33" s="110"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="111"/>
-      <c r="I33" s="111"/>
-      <c r="J33" s="111"/>
-      <c r="K33" s="111"/>
-    </row>
-    <row r="34" spans="2:11">
-      <c r="B34" s="110"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-    </row>
-    <row r="35" spans="2:11">
-      <c r="B35" s="110"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111"/>
-      <c r="J35" s="111"/>
-      <c r="K35" s="111"/>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="111"/>
-      <c r="F36" s="111"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-    </row>
-    <row r="37" spans="2:11">
-      <c r="B37" s="110"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-    </row>
-    <row r="38" spans="2:11">
-      <c r="B38" s="110"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-    </row>
-    <row r="39" spans="2:11">
-      <c r="B39" s="110"/>
-      <c r="C39" s="111"/>
-      <c r="D39" s="111"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="111"/>
-      <c r="H39" s="111"/>
-      <c r="I39" s="111"/>
-      <c r="J39" s="111"/>
-      <c r="K39" s="111"/>
-    </row>
-    <row r="40" spans="2:11">
-      <c r="B40" s="110"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-    </row>
-    <row r="41" spans="2:11">
-      <c r="B41" s="110"/>
-      <c r="C41" s="111" t="s">
+      <c r="E29" s="110"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="110"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="110"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="109"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="109"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="110"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="110"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="109"/>
+      <c r="C32" s="110"/>
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="109"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="110"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="110"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="109"/>
+      <c r="C34" s="110"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="110"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="109"/>
+      <c r="C35" s="110"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="110"/>
+      <c r="I35" s="110"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="110"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="109"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="110"/>
+      <c r="I36" s="110"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="110"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="109"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="110"/>
+      <c r="I37" s="110"/>
+      <c r="J37" s="110"/>
+      <c r="K37" s="110"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="109"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
+      <c r="E38" s="110"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
+      <c r="H38" s="110"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="110"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="109"/>
+      <c r="C39" s="110"/>
+      <c r="D39" s="110"/>
+      <c r="E39" s="110"/>
+      <c r="F39" s="110"/>
+      <c r="G39" s="110"/>
+      <c r="H39" s="110"/>
+      <c r="I39" s="110"/>
+      <c r="J39" s="110"/>
+      <c r="K39" s="110"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="109"/>
+      <c r="C40" s="110"/>
+      <c r="D40" s="110"/>
+      <c r="E40" s="110"/>
+      <c r="F40" s="110"/>
+      <c r="G40" s="110"/>
+      <c r="H40" s="110"/>
+      <c r="I40" s="110"/>
+      <c r="J40" s="110"/>
+      <c r="K40" s="110"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="109"/>
+      <c r="C41" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="111"/>
-      <c r="I41" s="111"/>
-      <c r="J41" s="111"/>
-      <c r="K41" s="111"/>
-    </row>
-    <row r="42" spans="2:11">
-      <c r="B42" s="110"/>
-      <c r="C42" s="111" t="s">
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="110"/>
+      <c r="G41" s="110"/>
+      <c r="H41" s="110"/>
+      <c r="I41" s="110"/>
+      <c r="J41" s="110"/>
+      <c r="K41" s="110"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="109"/>
+      <c r="C42" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="111"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="111"/>
-      <c r="G42" s="111"/>
-      <c r="H42" s="111"/>
-      <c r="I42" s="111"/>
-      <c r="J42" s="111"/>
-      <c r="K42" s="111"/>
-    </row>
-    <row r="43" spans="2:11">
-      <c r="B43" s="110"/>
-      <c r="C43" s="111"/>
-      <c r="D43" s="111"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="111"/>
-      <c r="G43" s="111"/>
-      <c r="H43" s="111"/>
-      <c r="I43" s="111"/>
-      <c r="J43" s="111"/>
-      <c r="K43" s="111"/>
-    </row>
-    <row r="44" spans="2:11">
-      <c r="B44" s="110"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="111"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="111"/>
-      <c r="G44" s="111"/>
-      <c r="H44" s="111"/>
-      <c r="I44" s="111"/>
-      <c r="J44" s="111"/>
-      <c r="K44" s="111"/>
-    </row>
-    <row r="45" spans="2:11">
-      <c r="B45" s="110"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-    </row>
-    <row r="46" spans="2:11">
-      <c r="B46" s="110"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-      <c r="J46" s="111"/>
-      <c r="K46" s="111"/>
-    </row>
-    <row r="47" spans="2:11">
-      <c r="B47" s="110"/>
-      <c r="C47" s="111">
+      <c r="D42" s="110"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="110"/>
+      <c r="G42" s="110"/>
+      <c r="H42" s="110"/>
+      <c r="I42" s="110"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="110"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="109"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="110"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="110"/>
+      <c r="G43" s="110"/>
+      <c r="H43" s="110"/>
+      <c r="I43" s="110"/>
+      <c r="J43" s="110"/>
+      <c r="K43" s="110"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="109"/>
+      <c r="C44" s="110"/>
+      <c r="D44" s="110"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="110"/>
+      <c r="G44" s="110"/>
+      <c r="H44" s="110"/>
+      <c r="I44" s="110"/>
+      <c r="J44" s="110"/>
+      <c r="K44" s="110"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="109"/>
+      <c r="C45" s="110"/>
+      <c r="D45" s="110"/>
+      <c r="E45" s="110"/>
+      <c r="F45" s="110"/>
+      <c r="G45" s="110"/>
+      <c r="H45" s="110"/>
+      <c r="I45" s="110"/>
+      <c r="J45" s="110"/>
+      <c r="K45" s="110"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46" s="109"/>
+      <c r="C46" s="110"/>
+      <c r="D46" s="110"/>
+      <c r="E46" s="110"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
+      <c r="I46" s="110"/>
+      <c r="J46" s="110"/>
+      <c r="K46" s="110"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" s="109"/>
+      <c r="C47" s="110">
         <v>74052</v>
       </c>
-      <c r="D47" s="111" t="s">
+      <c r="D47" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="111"/>
-      <c r="H47" s="111"/>
-      <c r="I47" s="111"/>
-      <c r="J47" s="111"/>
-      <c r="K47" s="111"/>
-    </row>
-    <row r="48" spans="2:11">
-      <c r="B48" s="110"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-      <c r="J48" s="111"/>
-      <c r="K48" s="111"/>
-    </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="110"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-      <c r="J49" s="111"/>
-      <c r="K49" s="111"/>
-    </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="110"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="111"/>
-    </row>
-    <row r="51" spans="2:11">
-      <c r="B51" s="110"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="111"/>
-    </row>
-    <row r="52" spans="2:11">
-      <c r="B52" s="110"/>
-      <c r="C52" s="111"/>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="111"/>
-      <c r="I52" s="111"/>
-      <c r="J52" s="111"/>
-      <c r="K52" s="111"/>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="B53" s="110"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="111"/>
-      <c r="E53" s="111"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="111"/>
-      <c r="I53" s="111"/>
-      <c r="J53" s="111"/>
-      <c r="K53" s="111"/>
-    </row>
-    <row r="54" spans="2:11">
-      <c r="B54" s="110"/>
-      <c r="C54" s="111">
+      <c r="E47" s="110"/>
+      <c r="F47" s="110"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="110"/>
+      <c r="I47" s="110"/>
+      <c r="J47" s="110"/>
+      <c r="K47" s="110"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="109"/>
+      <c r="C48" s="110"/>
+      <c r="D48" s="110"/>
+      <c r="E48" s="110"/>
+      <c r="F48" s="110"/>
+      <c r="G48" s="110"/>
+      <c r="H48" s="110"/>
+      <c r="I48" s="110"/>
+      <c r="J48" s="110"/>
+      <c r="K48" s="110"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="109"/>
+      <c r="C49" s="110"/>
+      <c r="D49" s="110"/>
+      <c r="E49" s="110"/>
+      <c r="F49" s="110"/>
+      <c r="G49" s="110"/>
+      <c r="H49" s="110"/>
+      <c r="I49" s="110"/>
+      <c r="J49" s="110"/>
+      <c r="K49" s="110"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="109"/>
+      <c r="C50" s="110"/>
+      <c r="D50" s="110"/>
+      <c r="E50" s="110"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="110"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="110"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B51" s="109"/>
+      <c r="C51" s="110"/>
+      <c r="D51" s="110"/>
+      <c r="E51" s="110"/>
+      <c r="F51" s="110"/>
+      <c r="G51" s="110"/>
+      <c r="H51" s="110"/>
+      <c r="I51" s="110"/>
+      <c r="J51" s="110"/>
+      <c r="K51" s="110"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="109"/>
+      <c r="C52" s="110"/>
+      <c r="D52" s="110"/>
+      <c r="E52" s="110"/>
+      <c r="F52" s="110"/>
+      <c r="G52" s="110"/>
+      <c r="H52" s="110"/>
+      <c r="I52" s="110"/>
+      <c r="J52" s="110"/>
+      <c r="K52" s="110"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="109"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="110"/>
+      <c r="E53" s="110"/>
+      <c r="F53" s="110"/>
+      <c r="G53" s="110"/>
+      <c r="H53" s="110"/>
+      <c r="I53" s="110"/>
+      <c r="J53" s="110"/>
+      <c r="K53" s="110"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="109"/>
+      <c r="C54" s="110">
         <v>3120</v>
       </c>
-      <c r="D54" s="111" t="s">
+      <c r="D54" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="111"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="111"/>
-      <c r="I54" s="111"/>
-      <c r="J54" s="111"/>
-      <c r="K54" s="111"/>
-    </row>
-    <row r="55" spans="2:11">
-      <c r="B55" s="110"/>
-      <c r="C55" s="111">
+      <c r="E54" s="110"/>
+      <c r="F54" s="110"/>
+      <c r="G54" s="110"/>
+      <c r="H54" s="110"/>
+      <c r="I54" s="110"/>
+      <c r="J54" s="110"/>
+      <c r="K54" s="110"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B55" s="109"/>
+      <c r="C55" s="110">
         <v>520</v>
       </c>
-      <c r="D55" s="111" t="s">
+      <c r="D55" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="111"/>
-      <c r="F55" s="111"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="111"/>
-      <c r="I55" s="111"/>
-      <c r="J55" s="111"/>
-      <c r="K55" s="111"/>
-    </row>
-    <row r="56" spans="2:11">
-      <c r="B56" s="110"/>
-      <c r="C56" s="111"/>
-      <c r="D56" s="111"/>
-      <c r="E56" s="111"/>
-      <c r="F56" s="111"/>
-      <c r="G56" s="111"/>
-      <c r="H56" s="111"/>
-      <c r="I56" s="111"/>
-      <c r="J56" s="111"/>
-      <c r="K56" s="111"/>
-    </row>
-    <row r="57" spans="2:11">
-      <c r="B57" s="110"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="111"/>
-      <c r="E57" s="111"/>
-      <c r="F57" s="111"/>
-      <c r="G57" s="111"/>
-      <c r="H57" s="111"/>
-      <c r="I57" s="111"/>
-      <c r="J57" s="111"/>
-      <c r="K57" s="111"/>
-    </row>
-    <row r="58" spans="2:11">
-      <c r="B58" s="110"/>
-      <c r="C58" s="111"/>
-      <c r="D58" s="111"/>
-      <c r="E58" s="111"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="111"/>
-      <c r="K58" s="111"/>
-    </row>
-    <row r="59" spans="2:11">
-      <c r="B59" s="110"/>
-      <c r="C59" s="111"/>
-      <c r="D59" s="111"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="111"/>
-      <c r="I59" s="111"/>
-      <c r="J59" s="111"/>
-      <c r="K59" s="111"/>
-    </row>
-    <row r="60" spans="2:11">
-      <c r="B60" s="110"/>
-      <c r="C60" s="111"/>
-      <c r="D60" s="111"/>
-      <c r="E60" s="111"/>
-      <c r="F60" s="111"/>
-      <c r="G60" s="111"/>
-      <c r="H60" s="111"/>
-      <c r="I60" s="111"/>
-      <c r="J60" s="111"/>
-      <c r="K60" s="111"/>
-    </row>
-    <row r="61" spans="2:11">
-      <c r="B61" s="110"/>
-      <c r="C61" s="111"/>
-      <c r="D61" s="111"/>
-      <c r="E61" s="111"/>
-      <c r="F61" s="111"/>
-      <c r="G61" s="111"/>
-      <c r="H61" s="111"/>
-      <c r="I61" s="111"/>
-      <c r="J61" s="111"/>
-      <c r="K61" s="111"/>
-    </row>
-    <row r="62" spans="2:11">
-      <c r="B62" s="110"/>
-      <c r="C62" s="111"/>
-      <c r="D62" s="111"/>
-      <c r="E62" s="111"/>
-      <c r="F62" s="111"/>
-      <c r="G62" s="111"/>
-      <c r="H62" s="111"/>
-      <c r="I62" s="111"/>
-      <c r="J62" s="111"/>
-      <c r="K62" s="111"/>
+      <c r="E55" s="110"/>
+      <c r="F55" s="110"/>
+      <c r="G55" s="110"/>
+      <c r="H55" s="110"/>
+      <c r="I55" s="110"/>
+      <c r="J55" s="110"/>
+      <c r="K55" s="110"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B56" s="109"/>
+      <c r="C56" s="110"/>
+      <c r="D56" s="110"/>
+      <c r="E56" s="110"/>
+      <c r="F56" s="110"/>
+      <c r="G56" s="110"/>
+      <c r="H56" s="110"/>
+      <c r="I56" s="110"/>
+      <c r="J56" s="110"/>
+      <c r="K56" s="110"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B57" s="109"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="110"/>
+      <c r="E57" s="110"/>
+      <c r="F57" s="110"/>
+      <c r="G57" s="110"/>
+      <c r="H57" s="110"/>
+      <c r="I57" s="110"/>
+      <c r="J57" s="110"/>
+      <c r="K57" s="110"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B58" s="109"/>
+      <c r="C58" s="110"/>
+      <c r="D58" s="110"/>
+      <c r="E58" s="110"/>
+      <c r="F58" s="110"/>
+      <c r="G58" s="110"/>
+      <c r="H58" s="110"/>
+      <c r="I58" s="110"/>
+      <c r="J58" s="110"/>
+      <c r="K58" s="110"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B59" s="109"/>
+      <c r="C59" s="110"/>
+      <c r="D59" s="110"/>
+      <c r="E59" s="110"/>
+      <c r="F59" s="110"/>
+      <c r="G59" s="110"/>
+      <c r="H59" s="110"/>
+      <c r="I59" s="110"/>
+      <c r="J59" s="110"/>
+      <c r="K59" s="110"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B60" s="109"/>
+      <c r="C60" s="110"/>
+      <c r="D60" s="110"/>
+      <c r="E60" s="110"/>
+      <c r="F60" s="110"/>
+      <c r="G60" s="110"/>
+      <c r="H60" s="110"/>
+      <c r="I60" s="110"/>
+      <c r="J60" s="110"/>
+      <c r="K60" s="110"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B61" s="109"/>
+      <c r="C61" s="110"/>
+      <c r="D61" s="110"/>
+      <c r="E61" s="110"/>
+      <c r="F61" s="110"/>
+      <c r="G61" s="110"/>
+      <c r="H61" s="110"/>
+      <c r="I61" s="110"/>
+      <c r="J61" s="110"/>
+      <c r="K61" s="110"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B62" s="109"/>
+      <c r="C62" s="110"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="110"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B63" s="109"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B64" s="109"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="109"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="109"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="109"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" s="109"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" s="109"/>
+      <c r="C69" s="123" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" s="106">
+        <v>9.4</v>
+      </c>
+      <c r="F69" s="123" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" s="109"/>
+      <c r="C70" s="123" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" s="106">
+        <f>1/E69</f>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="F70" s="123" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="109"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" s="109"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" s="109"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="109"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="109"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" s="109"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" s="109"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="109"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" s="109"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" s="109"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="109"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="109"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="109"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="109"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="109"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="109"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="109"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="109"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="109"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="109"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="109"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="109"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="109"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="109"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="109"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="109"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="109"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>